<commit_message>
Trabajando con cambios y errores en el sistema
</commit_message>
<xml_diff>
--- a/assets/files/beneficiarios.xlsx
+++ b/assets/files/beneficiarios.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\INSEZAC\Archivos de proyecto\Catalogos originales\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\INSEZAC\Archivos de proyecto\Catalogos pruebas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="109">
   <si>
     <t>CURP</t>
   </si>
@@ -164,6 +164,9 @@
     <t>AAAA830602MZSRVL02</t>
   </si>
   <si>
+    <t>ARANDA</t>
+  </si>
+  <si>
     <t>DE AVILA</t>
   </si>
   <si>
@@ -185,6 +188,9 @@
     <t>ALVARADO</t>
   </si>
   <si>
+    <t>BRENDA ALEJANDRA</t>
+  </si>
+  <si>
     <t>CERRO DE LA VIRGEN</t>
   </si>
   <si>
@@ -203,6 +209,9 @@
     <t>ANAYA</t>
   </si>
   <si>
+    <t>BRENDA PAOLA</t>
+  </si>
+  <si>
     <t>MATAMOROS</t>
   </si>
   <si>
@@ -225,6 +234,9 @@
   </si>
   <si>
     <t>AGUIRRE</t>
+  </si>
+  <si>
+    <t>DAVID</t>
   </si>
   <si>
     <t>IGNACIO ALVAREZ</t>
@@ -344,7 +356,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -764,8 +776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="Z14" sqref="Z14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -909,22 +921,22 @@
         <v>32</v>
       </c>
       <c r="AH1" s="2" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="AI1" s="2" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="AJ1" s="2" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="AK1" s="2" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="AL1" s="2" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="AM1" s="2" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.25">
@@ -956,10 +968,10 @@
         <v>0</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="L2" s="5" t="s">
         <v>38</v>
@@ -1028,7 +1040,7 @@
         <v>2</v>
       </c>
       <c r="AH2" s="8" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="AI2" s="9"/>
       <c r="AJ2" s="5">
@@ -1048,7 +1060,9 @@
       <c r="A3" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="5"/>
+      <c r="B3" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="C3" s="5" t="s">
         <v>41</v>
       </c>
@@ -1071,10 +1085,10 @@
         <v>123</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="L3" s="5" t="s">
         <v>38</v>
@@ -1143,7 +1157,7 @@
         <v>2</v>
       </c>
       <c r="AH3" s="8" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="AI3" s="9"/>
       <c r="AJ3" s="5">
@@ -1163,12 +1177,14 @@
       <c r="A4" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="5"/>
+      <c r="B4" s="5" t="s">
+        <v>46</v>
+      </c>
       <c r="C4" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E4" s="6">
         <v>1</v>
@@ -1177,7 +1193,7 @@
         <v>5</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H4" s="5">
         <v>149</v>
@@ -1186,16 +1202,16 @@
         <v>0</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="L4" s="5" t="s">
         <v>38</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N4" s="5">
         <v>2</v>
@@ -1258,7 +1274,7 @@
         <v>2</v>
       </c>
       <c r="AH4" s="8" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="AI4" s="9"/>
       <c r="AJ4" s="5">
@@ -1276,15 +1292,17 @@
     </row>
     <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D5" s="5"/>
+        <v>53</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>54</v>
+      </c>
       <c r="E5" s="6">
         <v>1</v>
       </c>
@@ -1292,25 +1310,25 @@
         <v>5</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="I5" s="5">
         <v>0</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="L5" s="5" t="s">
         <v>38</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="N5" s="5">
         <v>2</v>
@@ -1373,7 +1391,7 @@
         <v>2</v>
       </c>
       <c r="AH5" s="8" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="AI5" s="9"/>
       <c r="AJ5" s="5">
@@ -1391,23 +1409,25 @@
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D6" s="5"/>
+        <v>60</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>61</v>
+      </c>
       <c r="E6" s="6">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F6" s="6">
         <v>5</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="H6" s="5">
         <v>6</v>
@@ -1416,16 +1436,16 @@
         <v>0</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="L6" s="5" t="s">
         <v>38</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="N6" s="5">
         <v>2</v>
@@ -1488,7 +1508,7 @@
         <v>2</v>
       </c>
       <c r="AH6" s="8" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="AI6" s="9"/>
       <c r="AJ6" s="5">
@@ -1506,16 +1526,16 @@
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E7" s="6">
         <v>1</v>
@@ -1524,7 +1544,7 @@
         <v>5</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="H7" s="5">
         <v>6</v>
@@ -1533,16 +1553,16 @@
         <v>0</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="L7" s="5" t="s">
         <v>38</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="N7" s="5">
         <v>2</v>
@@ -1605,7 +1625,7 @@
         <v>2</v>
       </c>
       <c r="AH7" s="8" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="AI7" s="9"/>
       <c r="AJ7" s="5">
@@ -1623,15 +1643,17 @@
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>34</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D8" s="5"/>
+        <v>69</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>70</v>
+      </c>
       <c r="E8" s="6">
         <v>1</v>
       </c>
@@ -1639,7 +1661,7 @@
         <v>5</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="H8" s="5">
         <v>475</v>
@@ -1648,16 +1670,16 @@
         <v>0</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="L8" s="5" t="s">
         <v>38</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="N8" s="5">
         <v>2</v>
@@ -1720,7 +1742,7 @@
         <v>2</v>
       </c>
       <c r="AH8" s="8" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="AI8" s="9"/>
       <c r="AJ8" s="5">
@@ -1738,16 +1760,16 @@
     </row>
     <row r="9" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="E9" s="6">
         <v>1</v>
@@ -1756,7 +1778,7 @@
         <v>5</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="H9" s="5">
         <v>7</v>
@@ -1765,16 +1787,16 @@
         <v>0</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="L9" s="5" t="s">
         <v>38</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="N9" s="5">
         <v>2</v>
@@ -1837,7 +1859,7 @@
         <v>2</v>
       </c>
       <c r="AH9" s="8" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="AI9" s="9"/>
       <c r="AJ9" s="5">
@@ -1855,16 +1877,16 @@
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="E10" s="6">
         <v>1</v>
@@ -1873,7 +1895,7 @@
         <v>5</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="H10" s="5">
         <v>7</v>
@@ -1882,16 +1904,16 @@
         <v>0</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="L10" s="5" t="s">
         <v>38</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="N10" s="5">
         <v>2</v>
@@ -1954,7 +1976,7 @@
         <v>2</v>
       </c>
       <c r="AH10" s="8" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="AI10" s="9"/>
       <c r="AJ10" s="5">

</xml_diff>

<commit_message>
Cambios en el menu
</commit_message>
<xml_diff>
--- a/assets/files/beneficiarios.xlsx
+++ b/assets/files/beneficiarios.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\INSEZAC\Archivos de proyecto\Catalogos originales\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\INSEZAC\Archivos de proyecto\Catalogos pruebas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="109">
   <si>
     <t>CURP</t>
   </si>
@@ -164,6 +164,9 @@
     <t>AAAA830602MZSRVL02</t>
   </si>
   <si>
+    <t>ARANDA</t>
+  </si>
+  <si>
     <t>DE AVILA</t>
   </si>
   <si>
@@ -185,6 +188,9 @@
     <t>ALVARADO</t>
   </si>
   <si>
+    <t>BRENDA ALEJANDRA</t>
+  </si>
+  <si>
     <t>CERRO DE LA VIRGEN</t>
   </si>
   <si>
@@ -203,6 +209,9 @@
     <t>ANAYA</t>
   </si>
   <si>
+    <t>BRENDA PAOLA</t>
+  </si>
+  <si>
     <t>MATAMOROS</t>
   </si>
   <si>
@@ -225,6 +234,9 @@
   </si>
   <si>
     <t>AGUIRRE</t>
+  </si>
+  <si>
+    <t>DAVID</t>
   </si>
   <si>
     <t>IGNACIO ALVAREZ</t>
@@ -344,7 +356,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -764,8 +776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="Z14" sqref="Z14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -909,22 +921,22 @@
         <v>32</v>
       </c>
       <c r="AH1" s="2" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="AI1" s="2" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="AJ1" s="2" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="AK1" s="2" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="AL1" s="2" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="AM1" s="2" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.25">
@@ -956,10 +968,10 @@
         <v>0</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="L2" s="5" t="s">
         <v>38</v>
@@ -1028,7 +1040,7 @@
         <v>2</v>
       </c>
       <c r="AH2" s="8" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="AI2" s="9"/>
       <c r="AJ2" s="5">
@@ -1048,7 +1060,9 @@
       <c r="A3" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="5"/>
+      <c r="B3" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="C3" s="5" t="s">
         <v>41</v>
       </c>
@@ -1071,10 +1085,10 @@
         <v>123</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="L3" s="5" t="s">
         <v>38</v>
@@ -1143,7 +1157,7 @@
         <v>2</v>
       </c>
       <c r="AH3" s="8" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="AI3" s="9"/>
       <c r="AJ3" s="5">
@@ -1163,12 +1177,14 @@
       <c r="A4" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="5"/>
+      <c r="B4" s="5" t="s">
+        <v>46</v>
+      </c>
       <c r="C4" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E4" s="6">
         <v>1</v>
@@ -1177,7 +1193,7 @@
         <v>5</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H4" s="5">
         <v>149</v>
@@ -1186,16 +1202,16 @@
         <v>0</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="L4" s="5" t="s">
         <v>38</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N4" s="5">
         <v>2</v>
@@ -1258,7 +1274,7 @@
         <v>2</v>
       </c>
       <c r="AH4" s="8" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="AI4" s="9"/>
       <c r="AJ4" s="5">
@@ -1276,15 +1292,17 @@
     </row>
     <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D5" s="5"/>
+        <v>53</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>54</v>
+      </c>
       <c r="E5" s="6">
         <v>1</v>
       </c>
@@ -1292,25 +1310,25 @@
         <v>5</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="I5" s="5">
         <v>0</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="L5" s="5" t="s">
         <v>38</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="N5" s="5">
         <v>2</v>
@@ -1373,7 +1391,7 @@
         <v>2</v>
       </c>
       <c r="AH5" s="8" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="AI5" s="9"/>
       <c r="AJ5" s="5">
@@ -1391,23 +1409,25 @@
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D6" s="5"/>
+        <v>60</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>61</v>
+      </c>
       <c r="E6" s="6">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F6" s="6">
         <v>5</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="H6" s="5">
         <v>6</v>
@@ -1416,16 +1436,16 @@
         <v>0</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="L6" s="5" t="s">
         <v>38</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="N6" s="5">
         <v>2</v>
@@ -1488,7 +1508,7 @@
         <v>2</v>
       </c>
       <c r="AH6" s="8" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="AI6" s="9"/>
       <c r="AJ6" s="5">
@@ -1506,16 +1526,16 @@
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E7" s="6">
         <v>1</v>
@@ -1524,7 +1544,7 @@
         <v>5</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="H7" s="5">
         <v>6</v>
@@ -1533,16 +1553,16 @@
         <v>0</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="L7" s="5" t="s">
         <v>38</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="N7" s="5">
         <v>2</v>
@@ -1605,7 +1625,7 @@
         <v>2</v>
       </c>
       <c r="AH7" s="8" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="AI7" s="9"/>
       <c r="AJ7" s="5">
@@ -1623,15 +1643,17 @@
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>34</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D8" s="5"/>
+        <v>69</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>70</v>
+      </c>
       <c r="E8" s="6">
         <v>1</v>
       </c>
@@ -1639,7 +1661,7 @@
         <v>5</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="H8" s="5">
         <v>475</v>
@@ -1648,16 +1670,16 @@
         <v>0</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="L8" s="5" t="s">
         <v>38</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="N8" s="5">
         <v>2</v>
@@ -1720,7 +1742,7 @@
         <v>2</v>
       </c>
       <c r="AH8" s="8" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="AI8" s="9"/>
       <c r="AJ8" s="5">
@@ -1738,16 +1760,16 @@
     </row>
     <row r="9" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="E9" s="6">
         <v>1</v>
@@ -1756,7 +1778,7 @@
         <v>5</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="H9" s="5">
         <v>7</v>
@@ -1765,16 +1787,16 @@
         <v>0</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="L9" s="5" t="s">
         <v>38</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="N9" s="5">
         <v>2</v>
@@ -1837,7 +1859,7 @@
         <v>2</v>
       </c>
       <c r="AH9" s="8" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="AI9" s="9"/>
       <c r="AJ9" s="5">
@@ -1855,16 +1877,16 @@
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="E10" s="6">
         <v>1</v>
@@ -1873,7 +1895,7 @@
         <v>5</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="H10" s="5">
         <v>7</v>
@@ -1882,16 +1904,16 @@
         <v>0</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="L10" s="5" t="s">
         <v>38</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="N10" s="5">
         <v>2</v>
@@ -1954,7 +1976,7 @@
         <v>2</v>
       </c>
       <c r="AH10" s="8" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="AI10" s="9"/>
       <c r="AJ10" s="5">

</xml_diff>

<commit_message>
Agregue validacion de metodo importar en beneficiarios
</commit_message>
<xml_diff>
--- a/assets/files/beneficiarios.xlsx
+++ b/assets/files/beneficiarios.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\INSEZAC\Archivos de proyecto\Catalogos originales\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julieta\Dropbox\INSEZAC Residencias\Archivos de proyecto\Catalogos originales\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="115">
   <si>
     <t>CURP</t>
   </si>
@@ -164,6 +164,9 @@
     <t>AAAA830602MZSRVL02</t>
   </si>
   <si>
+    <t>ARANDA</t>
+  </si>
+  <si>
     <t>DE AVILA</t>
   </si>
   <si>
@@ -185,12 +188,12 @@
     <t>ALVARADO</t>
   </si>
   <si>
+    <t>BRENDA ALEJANDRA</t>
+  </si>
+  <si>
     <t>CERRO DE LA VIRGEN</t>
   </si>
   <si>
-    <t>6-B</t>
-  </si>
-  <si>
     <t>LOS PIRULES, GUADALUPE ,C.P. 98619</t>
   </si>
   <si>
@@ -203,6 +206,9 @@
     <t>ANAYA</t>
   </si>
   <si>
+    <t>BRENDA PAOLA</t>
+  </si>
+  <si>
     <t>MATAMOROS</t>
   </si>
   <si>
@@ -227,6 +233,9 @@
     <t>AGUIRRE</t>
   </si>
   <si>
+    <t>DAVID</t>
+  </si>
+  <si>
     <t>IGNACIO ALVAREZ</t>
   </si>
   <si>
@@ -339,12 +348,36 @@
   </si>
   <si>
     <t>Clave Municipio</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>ibarra</t>
+  </si>
+  <si>
+    <t>hernandez</t>
+  </si>
+  <si>
+    <t>AAAD980218MZSLGY06</t>
+  </si>
+  <si>
+    <t>hola</t>
+  </si>
+  <si>
+    <t>holi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -450,7 +483,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -476,7 +509,12 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
@@ -762,10 +800,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM10"/>
+  <dimension ref="A1:AM13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,14 +813,14 @@
     <col min="3" max="4" width="19.28515625" customWidth="1"/>
     <col min="5" max="5" width="23.42578125" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" customWidth="1"/>
     <col min="8" max="8" width="25" customWidth="1"/>
     <col min="9" max="9" width="20.5703125" customWidth="1"/>
     <col min="10" max="10" width="17.42578125" customWidth="1"/>
     <col min="11" max="11" width="22.28515625" customWidth="1"/>
     <col min="12" max="12" width="20.140625" customWidth="1"/>
     <col min="13" max="13" width="19.42578125" customWidth="1"/>
-    <col min="14" max="14" width="24.7109375" customWidth="1"/>
+    <col min="14" max="14" width="28.7109375" customWidth="1"/>
     <col min="15" max="15" width="24.28515625" customWidth="1"/>
     <col min="16" max="16" width="25.5703125" customWidth="1"/>
     <col min="18" max="18" width="11.5703125" bestFit="1" customWidth="1"/>
@@ -802,7 +840,7 @@
     <col min="34" max="34" width="25.28515625" customWidth="1"/>
     <col min="35" max="35" width="20.42578125" customWidth="1"/>
     <col min="36" max="36" width="17.140625" customWidth="1"/>
-    <col min="37" max="37" width="16.140625" customWidth="1"/>
+    <col min="37" max="37" width="26.7109375" customWidth="1"/>
     <col min="38" max="38" width="23.7109375" customWidth="1"/>
     <col min="39" max="39" width="18.5703125" customWidth="1"/>
     <col min="40" max="40" width="16.85546875" customWidth="1"/>
@@ -909,22 +947,22 @@
         <v>32</v>
       </c>
       <c r="AH1" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="AI1" s="2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="AJ1" s="2" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="AK1" s="2" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="AL1" s="2" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="AM1" s="2" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.25">
@@ -950,16 +988,16 @@
         <v>37</v>
       </c>
       <c r="H2" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I2" s="5">
         <v>0</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="L2" s="5" t="s">
         <v>38</v>
@@ -1028,11 +1066,13 @@
         <v>2</v>
       </c>
       <c r="AH2" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="AI2" s="9"/>
-      <c r="AJ2" s="5">
-        <v>1</v>
+        <v>102</v>
+      </c>
+      <c r="AI2" s="11">
+        <v>34768</v>
+      </c>
+      <c r="AJ2" s="10" t="s">
+        <v>108</v>
       </c>
       <c r="AK2" s="5">
         <v>2</v>
@@ -1048,7 +1088,9 @@
       <c r="A3" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="5"/>
+      <c r="B3" s="5" t="s">
+        <v>110</v>
+      </c>
       <c r="C3" s="5" t="s">
         <v>41</v>
       </c>
@@ -1071,10 +1113,10 @@
         <v>123</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="L3" s="5" t="s">
         <v>38</v>
@@ -1143,11 +1185,13 @@
         <v>2</v>
       </c>
       <c r="AH3" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="AI3" s="9"/>
-      <c r="AJ3" s="5">
-        <v>1</v>
+        <v>102</v>
+      </c>
+      <c r="AI3" s="11">
+        <v>34769</v>
+      </c>
+      <c r="AJ3" s="10" t="s">
+        <v>109</v>
       </c>
       <c r="AK3" s="5">
         <v>2</v>
@@ -1163,12 +1207,14 @@
       <c r="A4" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="5"/>
+      <c r="B4" s="5" t="s">
+        <v>46</v>
+      </c>
       <c r="C4" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E4" s="6">
         <v>1</v>
@@ -1177,7 +1223,7 @@
         <v>5</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H4" s="5">
         <v>149</v>
@@ -1186,16 +1232,16 @@
         <v>0</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="L4" s="5" t="s">
         <v>38</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N4" s="5">
         <v>2</v>
@@ -1258,11 +1304,13 @@
         <v>2</v>
       </c>
       <c r="AH4" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="AI4" s="9"/>
-      <c r="AJ4" s="5">
-        <v>1</v>
+        <v>102</v>
+      </c>
+      <c r="AI4" s="11">
+        <v>34770</v>
+      </c>
+      <c r="AJ4" s="10" t="s">
+        <v>108</v>
       </c>
       <c r="AK4" s="5">
         <v>2</v>
@@ -1276,15 +1324,17 @@
     </row>
     <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>51</v>
+        <v>111</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D5" s="5"/>
+        <v>53</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>54</v>
+      </c>
       <c r="E5" s="6">
         <v>1</v>
       </c>
@@ -1292,25 +1342,25 @@
         <v>5</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
+      </c>
+      <c r="H5" s="10">
+        <v>6</v>
       </c>
       <c r="I5" s="5">
         <v>0</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="L5" s="5" t="s">
         <v>38</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="N5" s="5">
         <v>2</v>
@@ -1373,11 +1423,13 @@
         <v>2</v>
       </c>
       <c r="AH5" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="AI5" s="9"/>
-      <c r="AJ5" s="5">
-        <v>1</v>
+        <v>102</v>
+      </c>
+      <c r="AI5" s="11">
+        <v>34771</v>
+      </c>
+      <c r="AJ5" s="10" t="s">
+        <v>109</v>
       </c>
       <c r="AK5" s="5">
         <v>2</v>
@@ -1391,23 +1443,25 @@
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D6" s="5"/>
+        <v>59</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>60</v>
+      </c>
       <c r="E6" s="6">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F6" s="6">
         <v>5</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H6" s="5">
         <v>6</v>
@@ -1416,16 +1470,16 @@
         <v>0</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="L6" s="5" t="s">
         <v>38</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="N6" s="5">
         <v>2</v>
@@ -1488,11 +1542,13 @@
         <v>2</v>
       </c>
       <c r="AH6" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="AI6" s="9"/>
-      <c r="AJ6" s="5">
-        <v>1</v>
+        <v>102</v>
+      </c>
+      <c r="AI6" s="11">
+        <v>34772</v>
+      </c>
+      <c r="AJ6" s="10" t="s">
+        <v>108</v>
       </c>
       <c r="AK6" s="5">
         <v>2</v>
@@ -1506,16 +1562,16 @@
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E7" s="6">
         <v>1</v>
@@ -1524,7 +1580,7 @@
         <v>5</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H7" s="5">
         <v>6</v>
@@ -1533,16 +1589,16 @@
         <v>0</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="L7" s="5" t="s">
         <v>38</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="N7" s="5">
         <v>2</v>
@@ -1605,11 +1661,13 @@
         <v>2</v>
       </c>
       <c r="AH7" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="AI7" s="9"/>
-      <c r="AJ7" s="5">
-        <v>1</v>
+        <v>102</v>
+      </c>
+      <c r="AI7" s="11">
+        <v>34773</v>
+      </c>
+      <c r="AJ7" s="10" t="s">
+        <v>109</v>
       </c>
       <c r="AK7" s="5">
         <v>2</v>
@@ -1623,15 +1681,17 @@
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>34</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D8" s="5"/>
+        <v>68</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>69</v>
+      </c>
       <c r="E8" s="6">
         <v>1</v>
       </c>
@@ -1639,7 +1699,7 @@
         <v>5</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="H8" s="5">
         <v>475</v>
@@ -1648,16 +1708,16 @@
         <v>0</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="L8" s="5" t="s">
         <v>38</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="N8" s="5">
         <v>2</v>
@@ -1720,11 +1780,13 @@
         <v>2</v>
       </c>
       <c r="AH8" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="AI8" s="9"/>
-      <c r="AJ8" s="5">
-        <v>1</v>
+        <v>102</v>
+      </c>
+      <c r="AI8" s="11">
+        <v>34774</v>
+      </c>
+      <c r="AJ8" s="10" t="s">
+        <v>108</v>
       </c>
       <c r="AK8" s="5">
         <v>2</v>
@@ -1738,16 +1800,16 @@
     </row>
     <row r="9" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E9" s="6">
         <v>1</v>
@@ -1756,7 +1818,7 @@
         <v>5</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="H9" s="5">
         <v>7</v>
@@ -1765,16 +1827,16 @@
         <v>0</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="L9" s="5" t="s">
         <v>38</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="N9" s="5">
         <v>2</v>
@@ -1837,11 +1899,13 @@
         <v>2</v>
       </c>
       <c r="AH9" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="AI9" s="9"/>
-      <c r="AJ9" s="5">
-        <v>1</v>
+        <v>102</v>
+      </c>
+      <c r="AI9" s="11">
+        <v>34955</v>
+      </c>
+      <c r="AJ9" s="10" t="s">
+        <v>109</v>
       </c>
       <c r="AK9" s="5">
         <v>2</v>
@@ -1855,16 +1919,16 @@
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="E10" s="6">
         <v>1</v>
@@ -1873,7 +1937,7 @@
         <v>5</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="H10" s="5">
         <v>7</v>
@@ -1882,16 +1946,16 @@
         <v>0</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="L10" s="5" t="s">
         <v>38</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="N10" s="5">
         <v>2</v>
@@ -1954,11 +2018,13 @@
         <v>2</v>
       </c>
       <c r="AH10" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="AI10" s="9"/>
-      <c r="AJ10" s="5">
-        <v>1</v>
+        <v>102</v>
+      </c>
+      <c r="AI10" s="11">
+        <v>34956</v>
+      </c>
+      <c r="AJ10" s="10" t="s">
+        <v>109</v>
       </c>
       <c r="AK10" s="5">
         <v>2</v>
@@ -1969,13 +2035,136 @@
       <c r="AM10" s="5">
         <v>9</v>
       </c>
+    </row>
+    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11" s="6">
+        <v>1</v>
+      </c>
+      <c r="F11" s="6">
+        <v>5</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="H11" s="5">
+        <v>7</v>
+      </c>
+      <c r="I11" s="5">
+        <v>0</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="N11" s="5">
+        <v>2</v>
+      </c>
+      <c r="O11" s="5">
+        <v>1</v>
+      </c>
+      <c r="P11" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q11" s="5">
+        <v>4</v>
+      </c>
+      <c r="R11" s="5">
+        <v>1</v>
+      </c>
+      <c r="S11" s="5">
+        <v>1</v>
+      </c>
+      <c r="T11" s="5">
+        <v>1</v>
+      </c>
+      <c r="U11" s="5">
+        <v>1</v>
+      </c>
+      <c r="V11" s="5">
+        <v>1</v>
+      </c>
+      <c r="W11" s="5">
+        <v>1</v>
+      </c>
+      <c r="X11" s="5">
+        <v>1</v>
+      </c>
+      <c r="Y11" s="5">
+        <v>1</v>
+      </c>
+      <c r="Z11" s="5">
+        <v>1</v>
+      </c>
+      <c r="AA11" s="5">
+        <v>1</v>
+      </c>
+      <c r="AB11" s="5">
+        <v>1</v>
+      </c>
+      <c r="AC11" s="5">
+        <v>4</v>
+      </c>
+      <c r="AD11" s="5">
+        <v>1</v>
+      </c>
+      <c r="AE11" s="5">
+        <v>1</v>
+      </c>
+      <c r="AF11" s="5">
+        <v>1</v>
+      </c>
+      <c r="AG11" s="5">
+        <v>2</v>
+      </c>
+      <c r="AH11" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="AI11" s="11">
+        <v>34956</v>
+      </c>
+      <c r="AJ11" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="AK11" s="5">
+        <v>2</v>
+      </c>
+      <c r="AL11" s="5">
+        <v>123456789</v>
+      </c>
+      <c r="AM11" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="F13" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="AH2" r:id="rId1"/>
     <hyperlink ref="AH3:AH10" r:id="rId2" display="example@hotmail.com"/>
+    <hyperlink ref="AH11" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Corregi los metodos de importar apoyosRFC, apoyosCURP, beneficiariosRFC
</commit_message>
<xml_diff>
--- a/assets/files/beneficiarios.xlsx
+++ b/assets/files/beneficiarios.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp2\htdocs\INSEZAC\Archivos de proyecto\Catalogos originales\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julieta\Dropbox\INSEZAC Residencias\Archivos de proyecto\Catalogos originales\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="115">
   <si>
     <t>CURP</t>
   </si>
@@ -164,6 +164,9 @@
     <t>AAAA830602MZSRVL02</t>
   </si>
   <si>
+    <t>ARANDA</t>
+  </si>
+  <si>
     <t>DE AVILA</t>
   </si>
   <si>
@@ -185,6 +188,9 @@
     <t>ALVARADO</t>
   </si>
   <si>
+    <t>BRENDA ALEJANDRA</t>
+  </si>
+  <si>
     <t>CERRO DE LA VIRGEN</t>
   </si>
   <si>
@@ -200,6 +206,9 @@
     <t>ANAYA</t>
   </si>
   <si>
+    <t>BRENDA PAOLA</t>
+  </si>
+  <si>
     <t>MATAMOROS</t>
   </si>
   <si>
@@ -209,6 +218,9 @@
     <t>AAAC420716MZSLLR02</t>
   </si>
   <si>
+    <t>MA DEL CARMEN</t>
+  </si>
+  <si>
     <t>URUGUAY</t>
   </si>
   <si>
@@ -221,6 +233,9 @@
     <t>AGUIRRE</t>
   </si>
   <si>
+    <t>DAVID</t>
+  </si>
+  <si>
     <t>IGNACIO ALVAREZ</t>
   </si>
   <si>
@@ -335,13 +350,34 @@
     <t>Clave Municipio</t>
   </si>
   <si>
-    <t>asdf</t>
+    <t>M</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>ibarra</t>
+  </si>
+  <si>
+    <t>hernandez</t>
+  </si>
+  <si>
+    <t>AAAD980218MZSLGY06</t>
+  </si>
+  <si>
+    <t>hola</t>
+  </si>
+  <si>
+    <t>holi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -447,7 +483,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -473,7 +509,12 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
@@ -759,10 +800,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM10"/>
+  <dimension ref="A1:AM13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -772,14 +813,14 @@
     <col min="3" max="4" width="19.28515625" customWidth="1"/>
     <col min="5" max="5" width="23.42578125" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" customWidth="1"/>
     <col min="8" max="8" width="25" customWidth="1"/>
     <col min="9" max="9" width="20.5703125" customWidth="1"/>
     <col min="10" max="10" width="17.42578125" customWidth="1"/>
     <col min="11" max="11" width="22.28515625" customWidth="1"/>
     <col min="12" max="12" width="20.140625" customWidth="1"/>
     <col min="13" max="13" width="19.42578125" customWidth="1"/>
-    <col min="14" max="14" width="24.7109375" customWidth="1"/>
+    <col min="14" max="14" width="28.7109375" customWidth="1"/>
     <col min="15" max="15" width="24.28515625" customWidth="1"/>
     <col min="16" max="16" width="25.5703125" customWidth="1"/>
     <col min="18" max="18" width="11.5703125" bestFit="1" customWidth="1"/>
@@ -799,7 +840,7 @@
     <col min="34" max="34" width="25.28515625" customWidth="1"/>
     <col min="35" max="35" width="20.42578125" customWidth="1"/>
     <col min="36" max="36" width="17.140625" customWidth="1"/>
-    <col min="37" max="37" width="16.140625" customWidth="1"/>
+    <col min="37" max="37" width="26.7109375" customWidth="1"/>
     <col min="38" max="38" width="23.7109375" customWidth="1"/>
     <col min="39" max="39" width="18.5703125" customWidth="1"/>
     <col min="40" max="40" width="16.85546875" customWidth="1"/>
@@ -906,22 +947,22 @@
         <v>32</v>
       </c>
       <c r="AH1" s="2" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="AI1" s="2" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="AJ1" s="2" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="AK1" s="2" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="AL1" s="2" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="AM1" s="2" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.25">
@@ -938,7 +979,7 @@
         <v>36</v>
       </c>
       <c r="E2" s="6">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F2" s="6">
         <v>5</v>
@@ -947,16 +988,16 @@
         <v>37</v>
       </c>
       <c r="H2" s="5">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="I2" s="5">
         <v>0</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="L2" s="5" t="s">
         <v>38</v>
@@ -1025,11 +1066,13 @@
         <v>2</v>
       </c>
       <c r="AH2" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="AI2" s="9"/>
-      <c r="AJ2" s="5">
-        <v>1</v>
+        <v>102</v>
+      </c>
+      <c r="AI2" s="11">
+        <v>34768</v>
+      </c>
+      <c r="AJ2" s="10" t="s">
+        <v>108</v>
       </c>
       <c r="AK2" s="5">
         <v>2</v>
@@ -1046,19 +1089,19 @@
         <v>40</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>34</v>
+        <v>110</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>41</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>70</v>
+        <v>42</v>
       </c>
       <c r="E3" s="6">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F3" s="6">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>43</v>
@@ -1070,10 +1113,10 @@
         <v>123</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="L3" s="5" t="s">
         <v>38</v>
@@ -1142,11 +1185,13 @@
         <v>2</v>
       </c>
       <c r="AH3" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="AI3" s="9"/>
-      <c r="AJ3" s="5">
-        <v>1</v>
+        <v>102</v>
+      </c>
+      <c r="AI3" s="11">
+        <v>34769</v>
+      </c>
+      <c r="AJ3" s="10" t="s">
+        <v>109</v>
       </c>
       <c r="AK3" s="5">
         <v>2</v>
@@ -1163,13 +1208,13 @@
         <v>45</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E4" s="6">
         <v>1</v>
@@ -1178,7 +1223,7 @@
         <v>5</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H4" s="5">
         <v>149</v>
@@ -1187,16 +1232,16 @@
         <v>0</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="L4" s="5" t="s">
         <v>38</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N4" s="5">
         <v>2</v>
@@ -1259,11 +1304,13 @@
         <v>2</v>
       </c>
       <c r="AH4" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="AI4" s="9"/>
-      <c r="AJ4" s="5">
-        <v>1</v>
+        <v>102</v>
+      </c>
+      <c r="AI4" s="11">
+        <v>34770</v>
+      </c>
+      <c r="AJ4" s="10" t="s">
+        <v>108</v>
       </c>
       <c r="AK4" s="5">
         <v>2</v>
@@ -1277,16 +1324,16 @@
     </row>
     <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>51</v>
+        <v>111</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E5" s="6">
         <v>1</v>
@@ -1295,25 +1342,25 @@
         <v>5</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="H5" s="5">
-        <v>3</v>
+        <v>55</v>
+      </c>
+      <c r="H5" s="10">
+        <v>6</v>
       </c>
       <c r="I5" s="5">
         <v>0</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="L5" s="5" t="s">
         <v>38</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="N5" s="5">
         <v>2</v>
@@ -1376,11 +1423,13 @@
         <v>2</v>
       </c>
       <c r="AH5" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="AI5" s="9"/>
-      <c r="AJ5" s="5">
-        <v>1</v>
+        <v>102</v>
+      </c>
+      <c r="AI5" s="11">
+        <v>34771</v>
+      </c>
+      <c r="AJ5" s="10" t="s">
+        <v>109</v>
       </c>
       <c r="AK5" s="5">
         <v>2</v>
@@ -1394,16 +1443,16 @@
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>103</v>
+        <v>60</v>
       </c>
       <c r="E6" s="6">
         <v>1</v>
@@ -1412,7 +1461,7 @@
         <v>5</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="H6" s="5">
         <v>6</v>
@@ -1421,16 +1470,16 @@
         <v>0</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="L6" s="5" t="s">
         <v>38</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="N6" s="5">
         <v>2</v>
@@ -1493,11 +1542,13 @@
         <v>2</v>
       </c>
       <c r="AH6" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="AI6" s="9"/>
-      <c r="AJ6" s="5">
-        <v>1</v>
+        <v>102</v>
+      </c>
+      <c r="AI6" s="11">
+        <v>34772</v>
+      </c>
+      <c r="AJ6" s="10" t="s">
+        <v>108</v>
       </c>
       <c r="AK6" s="5">
         <v>2</v>
@@ -1511,25 +1562,25 @@
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="E7" s="6">
         <v>1</v>
       </c>
       <c r="F7" s="6">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="H7" s="5">
         <v>6</v>
@@ -1538,16 +1589,16 @@
         <v>0</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="L7" s="5" t="s">
         <v>38</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="N7" s="5">
         <v>2</v>
@@ -1610,11 +1661,13 @@
         <v>2</v>
       </c>
       <c r="AH7" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="AI7" s="9"/>
-      <c r="AJ7" s="5">
-        <v>1</v>
+        <v>102</v>
+      </c>
+      <c r="AI7" s="11">
+        <v>34773</v>
+      </c>
+      <c r="AJ7" s="10" t="s">
+        <v>109</v>
       </c>
       <c r="AK7" s="5">
         <v>2</v>
@@ -1628,16 +1681,16 @@
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>34</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>47</v>
+        <v>69</v>
       </c>
       <c r="E8" s="6">
         <v>1</v>
@@ -1646,7 +1699,7 @@
         <v>5</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="H8" s="5">
         <v>475</v>
@@ -1655,16 +1708,16 @@
         <v>0</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="L8" s="5" t="s">
         <v>38</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="N8" s="5">
         <v>2</v>
@@ -1727,11 +1780,13 @@
         <v>2</v>
       </c>
       <c r="AH8" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="AI8" s="9"/>
-      <c r="AJ8" s="5">
-        <v>1</v>
+        <v>102</v>
+      </c>
+      <c r="AI8" s="11">
+        <v>34774</v>
+      </c>
+      <c r="AJ8" s="10" t="s">
+        <v>108</v>
       </c>
       <c r="AK8" s="5">
         <v>2</v>
@@ -1745,16 +1800,16 @@
     </row>
     <row r="9" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="E9" s="6">
         <v>1</v>
@@ -1763,7 +1818,7 @@
         <v>5</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="H9" s="5">
         <v>7</v>
@@ -1772,16 +1827,16 @@
         <v>0</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="L9" s="5" t="s">
         <v>38</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="N9" s="5">
         <v>2</v>
@@ -1844,11 +1899,13 @@
         <v>2</v>
       </c>
       <c r="AH9" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="AI9" s="9"/>
-      <c r="AJ9" s="5">
-        <v>1</v>
+        <v>102</v>
+      </c>
+      <c r="AI9" s="11">
+        <v>34955</v>
+      </c>
+      <c r="AJ9" s="10" t="s">
+        <v>109</v>
       </c>
       <c r="AK9" s="5">
         <v>2</v>
@@ -1862,16 +1919,16 @@
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="E10" s="6">
         <v>1</v>
@@ -1880,7 +1937,7 @@
         <v>5</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="H10" s="5">
         <v>7</v>
@@ -1889,16 +1946,16 @@
         <v>0</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="L10" s="5" t="s">
         <v>38</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="N10" s="5">
         <v>2</v>
@@ -1961,11 +2018,13 @@
         <v>2</v>
       </c>
       <c r="AH10" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="AI10" s="9"/>
-      <c r="AJ10" s="5">
-        <v>1</v>
+        <v>102</v>
+      </c>
+      <c r="AI10" s="11">
+        <v>34956</v>
+      </c>
+      <c r="AJ10" s="10" t="s">
+        <v>109</v>
       </c>
       <c r="AK10" s="5">
         <v>2</v>
@@ -1976,13 +2035,136 @@
       <c r="AM10" s="5">
         <v>9</v>
       </c>
+    </row>
+    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11" s="6">
+        <v>1</v>
+      </c>
+      <c r="F11" s="6">
+        <v>5</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="H11" s="5">
+        <v>7</v>
+      </c>
+      <c r="I11" s="5">
+        <v>0</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="N11" s="5">
+        <v>2</v>
+      </c>
+      <c r="O11" s="5">
+        <v>1</v>
+      </c>
+      <c r="P11" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q11" s="5">
+        <v>4</v>
+      </c>
+      <c r="R11" s="5">
+        <v>1</v>
+      </c>
+      <c r="S11" s="5">
+        <v>1</v>
+      </c>
+      <c r="T11" s="5">
+        <v>1</v>
+      </c>
+      <c r="U11" s="5">
+        <v>1</v>
+      </c>
+      <c r="V11" s="5">
+        <v>1</v>
+      </c>
+      <c r="W11" s="5">
+        <v>1</v>
+      </c>
+      <c r="X11" s="5">
+        <v>1</v>
+      </c>
+      <c r="Y11" s="5">
+        <v>1</v>
+      </c>
+      <c r="Z11" s="5">
+        <v>1</v>
+      </c>
+      <c r="AA11" s="5">
+        <v>1</v>
+      </c>
+      <c r="AB11" s="5">
+        <v>1</v>
+      </c>
+      <c r="AC11" s="5">
+        <v>4</v>
+      </c>
+      <c r="AD11" s="5">
+        <v>1</v>
+      </c>
+      <c r="AE11" s="5">
+        <v>1</v>
+      </c>
+      <c r="AF11" s="5">
+        <v>1</v>
+      </c>
+      <c r="AG11" s="5">
+        <v>2</v>
+      </c>
+      <c r="AH11" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="AI11" s="11">
+        <v>34956</v>
+      </c>
+      <c r="AJ11" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="AK11" s="5">
+        <v>2</v>
+      </c>
+      <c r="AL11" s="5">
+        <v>123456789</v>
+      </c>
+      <c r="AM11" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="F13" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="AH2" r:id="rId1"/>
     <hyperlink ref="AH3:AH10" r:id="rId2" display="example@hotmail.com"/>
+    <hyperlink ref="AH11" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>